<commit_message>
Docs:  update player profiles
Update player profiles.
</commit_message>
<xml_diff>
--- a/uefa_euro_2016_player_stats.xlsx
+++ b/uefa_euro_2016_player_stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="0" windowWidth="27560" windowHeight="16060" tabRatio="938"/>
+    <workbookView xWindow="140" yWindow="0" windowWidth="28500" windowHeight="16520" tabRatio="938"/>
   </bookViews>
   <sheets>
     <sheet name="player_data" sheetId="12" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="519">
   <si>
     <t>Antoine Griezmann</t>
   </si>
@@ -1556,12 +1556,33 @@
   <si>
     <t>Russia</t>
   </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1596,13 +1617,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1652,7 +1666,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="567">
+  <cellStyleXfs count="587">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2220,16 +2234,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="567">
+  <cellStyles count="587">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2513,6 +2546,16 @@
     <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2796,6 +2839,16 @@
     <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3127,9 +3180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B182" sqref="B182"/>
+      <selection pane="topRight" activeCell="B451" sqref="B451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3450,7 +3503,9 @@
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
@@ -3984,7 +4039,9 @@
       <c r="A7" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C7" s="2">
         <v>0</v>
       </c>
@@ -4518,7 +4575,9 @@
       <c r="A11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
@@ -5186,7 +5245,9 @@
       <c r="A16" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C16" s="2">
         <v>0</v>
       </c>
@@ -5452,7 +5513,9 @@
       <c r="A18" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C18" s="2">
         <v>0</v>
       </c>
@@ -5584,7 +5647,9 @@
       <c r="A19" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C19" s="2">
         <v>0</v>
       </c>
@@ -5716,7 +5781,9 @@
       <c r="A20" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C20" s="2">
         <v>0</v>
       </c>
@@ -5848,7 +5915,9 @@
       <c r="A21" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C21" s="2">
         <v>0</v>
       </c>
@@ -6650,7 +6719,9 @@
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C27" s="2">
         <v>3</v>
       </c>
@@ -6916,7 +6987,9 @@
       <c r="A29" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C29" s="2">
         <v>0</v>
       </c>
@@ -7718,7 +7791,9 @@
       <c r="A35" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C35" s="2">
         <v>0</v>
       </c>
@@ -7850,7 +7925,9 @@
       <c r="A36" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>514</v>
+      </c>
       <c r="C36" s="2">
         <v>0</v>
       </c>
@@ -8250,7 +8327,9 @@
       <c r="A39" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C39" s="2">
         <v>0</v>
       </c>
@@ -8382,7 +8461,9 @@
       <c r="A40" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C40" s="2">
         <v>0</v>
       </c>
@@ -8514,7 +8595,9 @@
       <c r="A41" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C41" s="2">
         <v>0</v>
       </c>
@@ -8646,7 +8729,9 @@
       <c r="A42" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C42" s="2">
         <v>0</v>
       </c>
@@ -9448,7 +9533,9 @@
       <c r="A48" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C48" s="2">
         <v>0</v>
       </c>
@@ -9714,7 +9801,9 @@
       <c r="A50" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C50" s="2">
         <v>0</v>
       </c>
@@ -10516,7 +10605,9 @@
       <c r="A56" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C56" s="2">
         <v>0</v>
       </c>
@@ -10648,7 +10739,9 @@
       <c r="A57" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C57" s="2">
         <v>0</v>
       </c>
@@ -10914,7 +11007,9 @@
       <c r="A59" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C59" s="2">
         <v>1</v>
       </c>
@@ -12118,7 +12213,9 @@
       <c r="A68" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B68" s="2"/>
+      <c r="B68" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C68" s="2">
         <v>0</v>
       </c>
@@ -12786,7 +12883,9 @@
       <c r="A73" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B73" s="2"/>
+      <c r="B73" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C73" s="2">
         <v>0</v>
       </c>
@@ -13052,7 +13151,9 @@
       <c r="A75" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B75" s="2"/>
+      <c r="B75" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C75" s="2">
         <v>0</v>
       </c>
@@ -13318,7 +13419,9 @@
       <c r="A77" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B77" s="2"/>
+      <c r="B77" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C77" s="2">
         <v>0</v>
       </c>
@@ -13584,7 +13687,9 @@
       <c r="A79" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B79" s="2"/>
+      <c r="B79" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C79" s="2">
         <v>0</v>
       </c>
@@ -13716,7 +13821,9 @@
       <c r="A80" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B80" s="2"/>
+      <c r="B80" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C80" s="2">
         <v>1</v>
       </c>
@@ -13982,7 +14089,9 @@
       <c r="A82" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B82" s="2"/>
+      <c r="B82" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C82" s="2">
         <v>0</v>
       </c>
@@ -14248,7 +14357,9 @@
       <c r="A84" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B84" s="2"/>
+      <c r="B84" s="2" t="s">
+        <v>516</v>
+      </c>
       <c r="C84" s="2">
         <v>0</v>
       </c>
@@ -14380,7 +14491,9 @@
       <c r="A85" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B85" s="2"/>
+      <c r="B85" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C85" s="2">
         <v>0</v>
       </c>
@@ -14512,7 +14625,9 @@
       <c r="A86" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="2"/>
+      <c r="B86" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C86" s="2">
         <v>0</v>
       </c>
@@ -14778,7 +14893,9 @@
       <c r="A88" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B88" s="2"/>
+      <c r="B88" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C88" s="2">
         <v>0</v>
       </c>
@@ -17322,7 +17439,9 @@
       <c r="A107" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B107" s="2"/>
+      <c r="B107" s="2" t="s">
+        <v>498</v>
+      </c>
       <c r="C107" s="2">
         <v>0</v>
       </c>
@@ -17722,7 +17841,9 @@
       <c r="A110" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B110" s="3"/>
+      <c r="B110" s="2" t="s">
+        <v>518</v>
+      </c>
       <c r="C110" s="2">
         <v>0</v>
       </c>
@@ -18390,7 +18511,9 @@
       <c r="A115" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B115" s="2"/>
+      <c r="B115" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C115" s="2">
         <v>0</v>
       </c>
@@ -18522,7 +18645,9 @@
       <c r="A116" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B116" s="2"/>
+      <c r="B116" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C116" s="2">
         <v>0</v>
       </c>
@@ -19056,7 +19181,9 @@
       <c r="A120" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B120" s="2"/>
+      <c r="B120" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C120" s="2">
         <v>0</v>
       </c>
@@ -19456,7 +19583,9 @@
       <c r="A123" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B123" s="2"/>
+      <c r="B123" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C123" s="2">
         <v>1</v>
       </c>
@@ -19588,7 +19717,9 @@
       <c r="A124" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B124" s="2"/>
+      <c r="B124" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C124" s="2">
         <v>0</v>
       </c>
@@ -19988,7 +20119,9 @@
       <c r="A127" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B127" s="2"/>
+      <c r="B127" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C127" s="2">
         <v>0</v>
       </c>
@@ -20656,7 +20789,9 @@
       <c r="A132" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B132" s="2"/>
+      <c r="B132" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C132" s="2">
         <v>0</v>
       </c>
@@ -21994,7 +22129,9 @@
       <c r="A142" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B142" s="2"/>
+      <c r="B142" s="2" t="s">
+        <v>514</v>
+      </c>
       <c r="C142" s="2">
         <v>0</v>
       </c>
@@ -22394,7 +22531,9 @@
       <c r="A145" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B145" s="2"/>
+      <c r="B145" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C145" s="2">
         <v>0</v>
       </c>
@@ -22526,7 +22665,9 @@
       <c r="A146" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B146" s="2"/>
+      <c r="B146" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C146" s="2">
         <v>0</v>
       </c>
@@ -22926,7 +23067,9 @@
       <c r="A149" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B149" s="2"/>
+      <c r="B149" s="2" t="s">
+        <v>514</v>
+      </c>
       <c r="C149" s="2">
         <v>0</v>
       </c>
@@ -23058,7 +23201,9 @@
       <c r="A150" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B150" s="2"/>
+      <c r="B150" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C150" s="2">
         <v>0</v>
       </c>
@@ -23458,7 +23603,9 @@
       <c r="A153" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B153" s="2"/>
+      <c r="B153" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C153" s="2">
         <v>0</v>
       </c>
@@ -23590,7 +23737,9 @@
       <c r="A154" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B154" s="2"/>
+      <c r="B154" s="2" t="s">
+        <v>515</v>
+      </c>
       <c r="C154" s="2">
         <v>1</v>
       </c>
@@ -23856,7 +24005,9 @@
       <c r="A156" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B156" s="2"/>
+      <c r="B156" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C156" s="2">
         <v>0</v>
       </c>
@@ -23988,7 +24139,9 @@
       <c r="A157" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B157" s="2"/>
+      <c r="B157" s="2" t="s">
+        <v>508</v>
+      </c>
       <c r="C157" s="2">
         <v>0</v>
       </c>
@@ -24790,7 +24943,9 @@
       <c r="A163" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B163" s="2"/>
+      <c r="B163" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C163" s="2">
         <v>3</v>
       </c>
@@ -25190,7 +25345,9 @@
       <c r="A166" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B166" s="2"/>
+      <c r="B166" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C166" s="2">
         <v>0</v>
       </c>
@@ -25322,7 +25479,9 @@
       <c r="A167" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B167" s="2"/>
+      <c r="B167" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C167" s="2">
         <v>0</v>
       </c>
@@ -25454,7 +25613,9 @@
       <c r="A168" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B168" s="2"/>
+      <c r="B168" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="C168" s="2">
         <v>1</v>
       </c>
@@ -26122,7 +26283,9 @@
       <c r="A173" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B173" s="2"/>
+      <c r="B173" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C173" s="2">
         <v>0</v>
       </c>
@@ -26388,7 +26551,9 @@
       <c r="A175" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B175" s="2"/>
+      <c r="B175" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C175" s="2">
         <v>0</v>
       </c>
@@ -26922,7 +27087,9 @@
       <c r="A179" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B179" s="2"/>
+      <c r="B179" s="2" t="s">
+        <v>516</v>
+      </c>
       <c r="C179" s="2">
         <v>0</v>
       </c>
@@ -27054,7 +27221,9 @@
       <c r="A180" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B180" s="2"/>
+      <c r="B180" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C180" s="2">
         <v>0</v>
       </c>
@@ -27186,7 +27355,9 @@
       <c r="A181" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B181" s="2"/>
+      <c r="B181" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C181" s="2">
         <v>2</v>
       </c>
@@ -27452,7 +27623,9 @@
       <c r="A183" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B183" s="2"/>
+      <c r="B183" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C183" s="2">
         <v>0</v>
       </c>
@@ -27852,7 +28025,7 @@
       <c r="A186" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B186" s="5" t="s">
+      <c r="B186" s="3" t="s">
         <v>511</v>
       </c>
       <c r="C186" s="2">
@@ -27986,7 +28159,9 @@
       <c r="A187" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B187" s="2"/>
+      <c r="B187" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C187" s="2">
         <v>0</v>
       </c>
@@ -28118,7 +28293,9 @@
       <c r="A188" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B188" s="2"/>
+      <c r="B188" s="2" t="s">
+        <v>516</v>
+      </c>
       <c r="C188" s="2">
         <v>0</v>
       </c>
@@ -29054,7 +29231,9 @@
       <c r="A195" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B195" s="2"/>
+      <c r="B195" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C195" s="2">
         <v>0</v>
       </c>
@@ -29186,7 +29365,9 @@
       <c r="A196" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B196" s="2"/>
+      <c r="B196" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C196" s="2">
         <v>0</v>
       </c>
@@ -29854,7 +30035,9 @@
       <c r="A201" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B201" s="2"/>
+      <c r="B201" s="2" t="s">
+        <v>507</v>
+      </c>
       <c r="C201" s="2">
         <v>0</v>
       </c>
@@ -29986,7 +30169,9 @@
       <c r="A202" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B202" s="2"/>
+      <c r="B202" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C202" s="2">
         <v>0</v>
       </c>
@@ -30118,7 +30303,9 @@
       <c r="A203" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B203" s="2"/>
+      <c r="B203" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C203" s="2">
         <v>0</v>
       </c>
@@ -30652,7 +30839,9 @@
       <c r="A207" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B207" s="2"/>
+      <c r="B207" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C207" s="2">
         <v>0</v>
       </c>
@@ -31052,7 +31241,9 @@
       <c r="A210" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B210" s="2"/>
+      <c r="B210" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C210" s="2">
         <v>0</v>
       </c>
@@ -31586,7 +31777,9 @@
       <c r="A214" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B214" s="2"/>
+      <c r="B214" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C214" s="2">
         <v>0</v>
       </c>
@@ -31852,7 +32045,9 @@
       <c r="A216" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B216" s="2"/>
+      <c r="B216" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C216" s="2">
         <v>0</v>
       </c>
@@ -31984,7 +32179,9 @@
       <c r="A217" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B217" s="2"/>
+      <c r="B217" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C217" s="2">
         <v>0</v>
       </c>
@@ -32250,7 +32447,9 @@
       <c r="A219" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B219" s="2"/>
+      <c r="B219" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C219" s="2">
         <v>0</v>
       </c>
@@ -32918,7 +33117,9 @@
       <c r="A224" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B224" s="2"/>
+      <c r="B224" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C224" s="2">
         <v>0</v>
       </c>
@@ -33452,7 +33653,9 @@
       <c r="A228" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B228" s="2"/>
+      <c r="B228" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C228" s="2">
         <v>0</v>
       </c>
@@ -34120,7 +34323,9 @@
       <c r="A233" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B233" s="2"/>
+      <c r="B233" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="C233" s="2">
         <v>0</v>
       </c>
@@ -34520,7 +34725,9 @@
       <c r="A236" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B236" s="2"/>
+      <c r="B236" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="C236" s="2">
         <v>0</v>
       </c>
@@ -35322,7 +35529,9 @@
       <c r="A242" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B242" s="2"/>
+      <c r="B242" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C242" s="2">
         <v>0</v>
       </c>
@@ -35588,7 +35797,9 @@
       <c r="A244" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B244" s="2"/>
+      <c r="B244" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C244" s="2">
         <v>0</v>
       </c>
@@ -35854,7 +36065,9 @@
       <c r="A246" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B246" s="2"/>
+      <c r="B246" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C246" s="2">
         <v>0</v>
       </c>
@@ -37728,7 +37941,9 @@
       <c r="A260" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B260" s="2"/>
+      <c r="B260" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C260" s="2">
         <v>0</v>
       </c>
@@ -38396,7 +38611,9 @@
       <c r="A265" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B265" s="2"/>
+      <c r="B265" s="2" t="s">
+        <v>508</v>
+      </c>
       <c r="C265" s="2">
         <v>0</v>
       </c>
@@ -39332,7 +39549,9 @@
       <c r="A272" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B272" s="2"/>
+      <c r="B272" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C272" s="2">
         <v>0</v>
       </c>
@@ -39598,7 +39817,9 @@
       <c r="A274" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B274" s="2"/>
+      <c r="B274" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C274" s="2">
         <v>1</v>
       </c>
@@ -40936,7 +41157,9 @@
       <c r="A284" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B284" s="2"/>
+      <c r="B284" s="2" t="s">
+        <v>514</v>
+      </c>
       <c r="C284" s="2">
         <v>0</v>
       </c>
@@ -41068,7 +41291,9 @@
       <c r="A285" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B285" s="2"/>
+      <c r="B285" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="C285" s="2">
         <v>0</v>
       </c>
@@ -41736,7 +41961,9 @@
       <c r="A290" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B290" s="2"/>
+      <c r="B290" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="C290" s="2">
         <v>0</v>
       </c>
@@ -41868,7 +42095,9 @@
       <c r="A291" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B291" s="2"/>
+      <c r="B291" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C291" s="2">
         <v>0</v>
       </c>
@@ -42268,7 +42497,9 @@
       <c r="A294" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B294" s="2"/>
+      <c r="B294" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C294" s="2">
         <v>0</v>
       </c>
@@ -42534,7 +42765,9 @@
       <c r="A296" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B296" s="2"/>
+      <c r="B296" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C296" s="2">
         <v>0</v>
       </c>
@@ -43336,7 +43569,9 @@
       <c r="A302" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B302" s="2"/>
+      <c r="B302" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C302" s="2">
         <v>0</v>
       </c>
@@ -43736,7 +43971,9 @@
       <c r="A305" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B305" s="2"/>
+      <c r="B305" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C305" s="2">
         <v>0</v>
       </c>
@@ -43868,7 +44105,9 @@
       <c r="A306" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B306" s="2"/>
+      <c r="B306" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C306" s="2">
         <v>0</v>
       </c>
@@ -44670,7 +44909,9 @@
       <c r="A312" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B312" s="2"/>
+      <c r="B312" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C312" s="2">
         <v>1</v>
       </c>
@@ -45338,7 +45579,9 @@
       <c r="A317" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B317" s="2"/>
+      <c r="B317" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C317" s="2">
         <v>1</v>
       </c>
@@ -45470,7 +45713,9 @@
       <c r="A318" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B318" s="2"/>
+      <c r="B318" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="C318" s="2">
         <v>0</v>
       </c>
@@ -45602,7 +45847,9 @@
       <c r="A319" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B319" s="2"/>
+      <c r="B319" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C319" s="2">
         <v>0</v>
       </c>
@@ -45868,7 +46115,9 @@
       <c r="A321" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B321" s="2"/>
+      <c r="B321" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C321" s="2">
         <v>0</v>
       </c>
@@ -46000,7 +46249,9 @@
       <c r="A322" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B322" s="2"/>
+      <c r="B322" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C322" s="2">
         <v>0</v>
       </c>
@@ -46132,7 +46383,9 @@
       <c r="A323" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B323" s="2"/>
+      <c r="B323" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C323" s="2">
         <v>0</v>
       </c>
@@ -46264,7 +46517,9 @@
       <c r="A324" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B324" s="2"/>
+      <c r="B324" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C324" s="2">
         <v>0</v>
       </c>
@@ -46396,7 +46651,9 @@
       <c r="A325" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B325" s="2"/>
+      <c r="B325" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C325" s="2">
         <v>0</v>
       </c>
@@ -46796,7 +47053,9 @@
       <c r="A328" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B328" s="2"/>
+      <c r="B328" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C328" s="2">
         <v>1</v>
       </c>
@@ -46928,7 +47187,9 @@
       <c r="A329" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B329" s="2"/>
+      <c r="B329" s="2" t="s">
+        <v>514</v>
+      </c>
       <c r="C329" s="2">
         <v>0</v>
       </c>
@@ -47194,7 +47455,9 @@
       <c r="A331" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B331" s="2"/>
+      <c r="B331" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C331" s="2">
         <v>1</v>
       </c>
@@ -47594,7 +47857,9 @@
       <c r="A334" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B334" s="2"/>
+      <c r="B334" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C334" s="2">
         <v>0</v>
       </c>
@@ -47994,7 +48259,9 @@
       <c r="A337" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B337" s="2"/>
+      <c r="B337" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C337" s="2">
         <v>0</v>
       </c>
@@ -48126,7 +48393,9 @@
       <c r="A338" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B338" s="2"/>
+      <c r="B338" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C338" s="2">
         <v>0</v>
       </c>
@@ -48392,7 +48661,9 @@
       <c r="A340" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B340" s="2"/>
+      <c r="B340" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C340" s="2">
         <v>0</v>
       </c>
@@ -48524,7 +48795,9 @@
       <c r="A341" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B341" s="2"/>
+      <c r="B341" s="2" t="s">
+        <v>499</v>
+      </c>
       <c r="C341" s="2">
         <v>0</v>
       </c>
@@ -49996,7 +50269,9 @@
       <c r="A352" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B352" s="2"/>
+      <c r="B352" s="2" t="s">
+        <v>515</v>
+      </c>
       <c r="C352" s="2">
         <v>0</v>
       </c>
@@ -50932,7 +51207,9 @@
       <c r="A359" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B359" s="2"/>
+      <c r="B359" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C359" s="2">
         <v>0</v>
       </c>
@@ -51332,7 +51609,9 @@
       <c r="A362" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B362" s="2"/>
+      <c r="B362" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C362" s="2">
         <v>0</v>
       </c>
@@ -51464,7 +51743,9 @@
       <c r="A363" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B363" s="2"/>
+      <c r="B363" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C363" s="2">
         <v>0</v>
       </c>
@@ -51596,7 +51877,9 @@
       <c r="A364" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B364" s="2"/>
+      <c r="B364" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C364" s="2">
         <v>0</v>
       </c>
@@ -52130,7 +52413,9 @@
       <c r="A368" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B368" s="2"/>
+      <c r="B368" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C368" s="2">
         <v>0</v>
       </c>
@@ -52530,7 +52815,9 @@
       <c r="A371" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B371" s="2"/>
+      <c r="B371" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C371" s="2">
         <v>1</v>
       </c>
@@ -53064,7 +53351,9 @@
       <c r="A375" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B375" s="2"/>
+      <c r="B375" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C375" s="2">
         <v>0</v>
       </c>
@@ -53330,7 +53619,9 @@
       <c r="A377" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B377" s="2"/>
+      <c r="B377" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C377" s="2">
         <v>0</v>
       </c>
@@ -53462,7 +53753,9 @@
       <c r="A378" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B378" s="2"/>
+      <c r="B378" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C378" s="2">
         <v>0</v>
       </c>
@@ -53594,7 +53887,9 @@
       <c r="A379" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B379" s="2"/>
+      <c r="B379" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C379" s="2">
         <v>0</v>
       </c>
@@ -53726,7 +54021,9 @@
       <c r="A380" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B380" s="2"/>
+      <c r="B380" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C380" s="2">
         <v>0</v>
       </c>
@@ -53858,7 +54155,9 @@
       <c r="A381" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B381" s="2"/>
+      <c r="B381" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C381" s="2">
         <v>0</v>
       </c>
@@ -54392,7 +54691,9 @@
       <c r="A385" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B385" s="2"/>
+      <c r="B385" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C385" s="2">
         <v>0</v>
       </c>
@@ -54926,7 +55227,9 @@
       <c r="A389" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B389" s="2"/>
+      <c r="B389" s="3" t="s">
+        <v>518</v>
+      </c>
       <c r="C389" s="2">
         <v>0</v>
       </c>
@@ -55460,7 +55763,9 @@
       <c r="A393" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B393" s="2"/>
+      <c r="B393" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C393" s="2">
         <v>0</v>
       </c>
@@ -56128,7 +56433,9 @@
       <c r="A398" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B398" s="2"/>
+      <c r="B398" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C398" s="2">
         <v>0</v>
       </c>
@@ -57198,7 +57505,9 @@
       <c r="A406" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B406" s="2"/>
+      <c r="B406" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C406" s="2">
         <v>0</v>
       </c>
@@ -57590,7 +57899,9 @@
       <c r="A409" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B409" s="2"/>
+      <c r="B409" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C409" s="2">
         <v>0</v>
       </c>
@@ -58794,7 +59105,9 @@
       <c r="A418" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B418" s="2"/>
+      <c r="B418" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C418" s="2">
         <v>0</v>
       </c>
@@ -59596,7 +59909,9 @@
       <c r="A424" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B424" s="2"/>
+      <c r="B424" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C424" s="2">
         <v>0</v>
       </c>
@@ -59728,7 +60043,9 @@
       <c r="A425" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B425" s="2"/>
+      <c r="B425" s="3" t="s">
+        <v>511</v>
+      </c>
       <c r="C425" s="2">
         <v>1</v>
       </c>
@@ -59994,7 +60311,9 @@
       <c r="A427" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B427" s="2"/>
+      <c r="B427" s="2" t="s">
+        <v>514</v>
+      </c>
       <c r="C427" s="2">
         <v>0</v>
       </c>
@@ -60260,7 +60579,9 @@
       <c r="A429" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="B429" s="2"/>
+      <c r="B429" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C429" s="2">
         <v>0</v>
       </c>
@@ -60392,7 +60713,9 @@
       <c r="A430" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B430" s="2"/>
+      <c r="B430" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C430" s="2">
         <v>0</v>
       </c>
@@ -60792,7 +61115,9 @@
       <c r="A433" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B433" s="2"/>
+      <c r="B433" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="C433" s="2">
         <v>1</v>
       </c>
@@ -60924,7 +61249,9 @@
       <c r="A434" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B434" s="2"/>
+      <c r="B434" s="2" t="s">
+        <v>516</v>
+      </c>
       <c r="C434" s="2">
         <v>0</v>
       </c>
@@ -61056,7 +61383,9 @@
       <c r="A435" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B435" s="2"/>
+      <c r="B435" s="3" t="s">
+        <v>516</v>
+      </c>
       <c r="C435" s="2">
         <v>0</v>
       </c>
@@ -61188,7 +61517,9 @@
       <c r="A436" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B436" s="2"/>
+      <c r="B436" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C436" s="2">
         <v>0</v>
       </c>
@@ -61320,7 +61651,9 @@
       <c r="A437" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B437" s="2"/>
+      <c r="B437" s="2" t="s">
+        <v>518</v>
+      </c>
       <c r="C437" s="2">
         <v>0</v>
       </c>
@@ -61988,7 +62321,9 @@
       <c r="A442" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B442" s="2"/>
+      <c r="B442" s="3" t="s">
+        <v>515</v>
+      </c>
       <c r="C442" s="2">
         <v>1</v>
       </c>
@@ -62120,7 +62455,9 @@
       <c r="A443" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B443" s="2"/>
+      <c r="B443" s="2" t="s">
+        <v>515</v>
+      </c>
       <c r="C443" s="2">
         <v>0</v>
       </c>
@@ -62386,7 +62723,9 @@
       <c r="A445" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B445" s="2"/>
+      <c r="B445" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C445" s="2">
         <v>0</v>
       </c>
@@ -62518,7 +62857,9 @@
       <c r="A446" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B446" s="2"/>
+      <c r="B446" s="2" t="s">
+        <v>517</v>
+      </c>
       <c r="C446" s="2">
         <v>0</v>
       </c>
@@ -62650,7 +62991,9 @@
       <c r="A447" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B447" s="2"/>
+      <c r="B447" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C447" s="2">
         <v>0</v>
       </c>
@@ -62782,7 +63125,9 @@
       <c r="A448" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B448" s="2"/>
+      <c r="B448" s="3" t="s">
+        <v>517</v>
+      </c>
       <c r="C448" s="2">
         <v>0</v>
       </c>
@@ -63048,7 +63393,9 @@
       <c r="A450" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B450" s="2"/>
+      <c r="B450" s="2" t="s">
+        <v>516</v>
+      </c>
       <c r="C450" s="2">
         <v>0</v>
       </c>
@@ -63180,7 +63527,9 @@
       <c r="A451" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B451" s="2"/>
+      <c r="B451" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C451" s="2">
         <v>0</v>
       </c>
@@ -63711,7 +64060,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>